<commit_message>
[#95] - add frontend datas
</commit_message>
<xml_diff>
--- a/analytics-raw-data/data/fga-eps-mds-2021_1-Cartografia-Social-ANALYSYS.xlsx
+++ b/analytics-raw-data/data/fga-eps-mds-2021_1-Cartografia-Social-ANALYSYS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>m1</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Cartografia-social-api-users</t>
   </si>
   <si>
+    <t>Cartografia-social-api-front</t>
+  </si>
+  <si>
     <t>v0.0.1</t>
   </si>
   <si>
@@ -110,6 +113,18 @@
   </si>
   <si>
     <t>v1.0.2</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>v1.1.0</t>
+  </si>
+  <si>
+    <t>v1.1.1</t>
+  </si>
+  <si>
+    <t>v1.1.2</t>
   </si>
 </sst>
 </file>
@@ -467,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2">
         <v>336</v>
@@ -584,7 +599,7 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3">
         <v>161</v>
@@ -628,7 +643,7 @@
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4">
         <v>196</v>
@@ -672,7 +687,7 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5">
         <v>284</v>
@@ -716,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6">
         <v>334</v>
@@ -760,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7">
         <v>393</v>
@@ -804,7 +819,7 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8">
         <v>480</v>
@@ -848,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I9">
         <v>482</v>
@@ -892,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I10">
         <v>1031</v>
@@ -936,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I11">
         <v>429</v>
@@ -980,7 +995,7 @@
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12">
         <v>1031</v>
@@ -1024,7 +1039,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13">
         <v>46</v>
@@ -1068,7 +1083,7 @@
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I14">
         <v>121</v>
@@ -1112,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15">
         <v>184</v>
@@ -1156,7 +1171,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I16">
         <v>239</v>
@@ -1200,7 +1215,7 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I17">
         <v>282</v>
@@ -1244,7 +1259,7 @@
         <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I18">
         <v>367</v>
@@ -1288,7 +1303,7 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I19">
         <v>367</v>
@@ -1332,7 +1347,7 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I20">
         <v>450</v>
@@ -1376,7 +1391,7 @@
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I21">
         <v>462</v>
@@ -1420,7 +1435,7 @@
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I22">
         <v>551</v>
@@ -1464,7 +1479,7 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I23">
         <v>214</v>
@@ -1508,7 +1523,7 @@
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I24">
         <v>167</v>
@@ -1552,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I25">
         <v>419</v>
@@ -1596,7 +1611,7 @@
         <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I26">
         <v>556</v>
@@ -1640,7 +1655,7 @@
         <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I27">
         <v>560</v>
@@ -1684,7 +1699,7 @@
         <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I28">
         <v>162</v>
@@ -1728,7 +1743,7 @@
         <v>17</v>
       </c>
       <c r="H29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I29">
         <v>148</v>
@@ -1772,7 +1787,7 @@
         <v>17</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I30">
         <v>151</v>
@@ -1816,7 +1831,7 @@
         <v>18</v>
       </c>
       <c r="H31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I31">
         <v>601</v>
@@ -1835,6 +1850,622 @@
       </c>
       <c r="N31">
         <v>0.8064285714285715</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>0.8181818181818182</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32">
+        <v>1921</v>
+      </c>
+      <c r="J32">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>0.3</v>
+      </c>
+      <c r="M32">
+        <v>0.5</v>
+      </c>
+      <c r="N32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>0.6909090909090909</v>
+      </c>
+      <c r="B33">
+        <v>0.03636363636363636</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33">
+        <v>1412</v>
+      </c>
+      <c r="J33">
+        <v>0.5700000000000001</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>0.285</v>
+      </c>
+      <c r="M33">
+        <v>0.5</v>
+      </c>
+      <c r="N33">
+        <v>0.785</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>0.6909090909090909</v>
+      </c>
+      <c r="B34">
+        <v>0.03636363636363636</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34">
+        <v>1412</v>
+      </c>
+      <c r="J34">
+        <v>0.5700000000000001</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>0.285</v>
+      </c>
+      <c r="M34">
+        <v>0.5</v>
+      </c>
+      <c r="N34">
+        <v>0.785</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>0.6</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35">
+        <v>525</v>
+      </c>
+      <c r="J35">
+        <v>0.528</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0.264</v>
+      </c>
+      <c r="M35">
+        <v>0.5</v>
+      </c>
+      <c r="N35">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>0.6</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36">
+        <v>525</v>
+      </c>
+      <c r="J36">
+        <v>0.528</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>0.264</v>
+      </c>
+      <c r="M36">
+        <v>0.5</v>
+      </c>
+      <c r="N36">
+        <v>0.764</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="D37">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="E37">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="F37">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37">
+        <v>975</v>
+      </c>
+      <c r="J37">
+        <v>0.55</v>
+      </c>
+      <c r="K37">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="L37">
+        <v>0.275</v>
+      </c>
+      <c r="M37">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="N37">
+        <v>0.7472222222222222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>0.75</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0.95</v>
+      </c>
+      <c r="D38">
+        <v>0.95</v>
+      </c>
+      <c r="E38">
+        <v>0.95</v>
+      </c>
+      <c r="F38">
+        <v>0.95</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38">
+        <v>1077</v>
+      </c>
+      <c r="J38">
+        <v>0.5609999999999999</v>
+      </c>
+      <c r="K38">
+        <v>0.95</v>
+      </c>
+      <c r="L38">
+        <v>0.2805</v>
+      </c>
+      <c r="M38">
+        <v>0.475</v>
+      </c>
+      <c r="N38">
+        <v>0.7554999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>0.8148148148148148</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39">
+        <v>1625</v>
+      </c>
+      <c r="J39">
+        <v>0.5988888888888889</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>0.2994444444444445</v>
+      </c>
+      <c r="M39">
+        <v>0.5</v>
+      </c>
+      <c r="N39">
+        <v>0.7994444444444444</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40">
+        <v>1788</v>
+      </c>
+      <c r="J40">
+        <v>0.605</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>0.3025</v>
+      </c>
+      <c r="M40">
+        <v>0.5</v>
+      </c>
+      <c r="N40">
+        <v>0.8025</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>0.8285714285714286</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="D41">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="E41">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="F41">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41">
+        <v>2086</v>
+      </c>
+      <c r="J41">
+        <v>0.5845714285714286</v>
+      </c>
+      <c r="K41">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="L41">
+        <v>0.2922857142857143</v>
+      </c>
+      <c r="M41">
+        <v>0.4714285714285714</v>
+      </c>
+      <c r="N41">
+        <v>0.7637142857142858</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="D42">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="E42">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="F42">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42">
+        <v>2136</v>
+      </c>
+      <c r="J42">
+        <v>0.5866666666666667</v>
+      </c>
+      <c r="K42">
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="L42">
+        <v>0.2933333333333333</v>
+      </c>
+      <c r="M42">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="N42">
+        <v>0.7655555555555555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="D43">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="E43">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="F43">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43">
+        <v>3091</v>
+      </c>
+      <c r="J43">
+        <v>0.5584615384615386</v>
+      </c>
+      <c r="K43">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="L43">
+        <v>0.2792307692307693</v>
+      </c>
+      <c r="M43">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="N43">
+        <v>0.7407692307692308</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D44">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="E44">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F44">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G44" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44">
+        <v>3545</v>
+      </c>
+      <c r="J44">
+        <v>0.5657142857142857</v>
+      </c>
+      <c r="K44">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="L44">
+        <v>0.2828571428571429</v>
+      </c>
+      <c r="M44">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="N44">
+        <v>0.7471428571428571</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D45">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="E45">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F45">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I45">
+        <v>3511</v>
+      </c>
+      <c r="J45">
+        <v>0.5657142857142857</v>
+      </c>
+      <c r="K45">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="L45">
+        <v>0.2828571428571429</v>
+      </c>
+      <c r="M45">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="N45">
+        <v>0.7471428571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[95] docs - add histogram chart
</commit_message>
<xml_diff>
--- a/analytics-raw-data/data/fga-eps-mds-2021_1-Cartografia-Social-ANALYSYS.xlsx
+++ b/analytics-raw-data/data/fga-eps-mds-2021_1-Cartografia-Social-ANALYSYS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
   <si>
     <t>m1</t>
   </si>
@@ -118,6 +118,15 @@
     <t>MVP</t>
   </si>
   <si>
+    <t>v1.0.3</t>
+  </si>
+  <si>
+    <t>v1.0.4</t>
+  </si>
+  <si>
+    <t>v1.0.5</t>
+  </si>
+  <si>
     <t>v1.1.0</t>
   </si>
   <si>
@@ -125,6 +134,12 @@
   </si>
   <si>
     <t>v1.1.2</t>
+  </si>
+  <si>
+    <t>v2.0.0</t>
+  </si>
+  <si>
+    <t>v2.0.1</t>
   </si>
 </sst>
 </file>
@@ -482,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2338,134 +2353,398 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43">
-        <v>0.7692307692307693</v>
+        <v>0.8043478260869565</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0.9230769230769231</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="D43">
-        <v>0.9230769230769231</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="E43">
-        <v>0.9230769230769231</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="F43">
-        <v>0.9230769230769231</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="G43" t="s">
         <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I43">
-        <v>3091</v>
+        <v>2657</v>
       </c>
       <c r="J43">
-        <v>0.5584615384615386</v>
+        <v>0.5810869565217391</v>
       </c>
       <c r="K43">
-        <v>0.9230769230769231</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="L43">
-        <v>0.2792307692307693</v>
+        <v>0.2905434782608696</v>
       </c>
       <c r="M43">
-        <v>0.4615384615384616</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="N43">
-        <v>0.7407692307692308</v>
+        <v>0.768804347826087</v>
       </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44">
-        <v>0.7857142857142857</v>
+        <v>0.8</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0.9285714285714286</v>
+        <v>0.96</v>
       </c>
       <c r="D44">
-        <v>0.9285714285714286</v>
+        <v>0.96</v>
       </c>
       <c r="E44">
-        <v>0.9285714285714286</v>
+        <v>0.96</v>
       </c>
       <c r="F44">
-        <v>0.9285714285714286</v>
+        <v>0.96</v>
       </c>
       <c r="G44" t="s">
         <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I44">
-        <v>3545</v>
+        <v>2893</v>
       </c>
       <c r="J44">
-        <v>0.5657142857142857</v>
+        <v>0.5808</v>
       </c>
       <c r="K44">
-        <v>0.9285714285714286</v>
+        <v>0.96</v>
       </c>
       <c r="L44">
-        <v>0.2828571428571429</v>
+        <v>0.2904</v>
       </c>
       <c r="M44">
-        <v>0.4642857142857143</v>
+        <v>0.48</v>
       </c>
       <c r="N44">
-        <v>0.7471428571428571</v>
+        <v>0.7704</v>
       </c>
     </row>
     <row r="45" spans="1:14">
       <c r="A45">
-        <v>0.7857142857142857</v>
+        <v>0.7884615384615384</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>0.9285714285714286</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="D45">
-        <v>0.9285714285714286</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E45">
-        <v>0.9285714285714286</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="F45">
-        <v>0.9285714285714286</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="G45" t="s">
         <v>19</v>
       </c>
       <c r="H45" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45">
+        <v>3057</v>
+      </c>
+      <c r="J45">
+        <v>0.5648076923076923</v>
+      </c>
+      <c r="K45">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="L45">
+        <v>0.2824038461538462</v>
+      </c>
+      <c r="M45">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="N45">
+        <v>0.7439423076923077</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="D46">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="E46">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="F46">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
         <v>36</v>
       </c>
-      <c r="I45">
+      <c r="I46">
+        <v>3091</v>
+      </c>
+      <c r="J46">
+        <v>0.5584615384615386</v>
+      </c>
+      <c r="K46">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="L46">
+        <v>0.2792307692307693</v>
+      </c>
+      <c r="M46">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="N46">
+        <v>0.7407692307692308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="D47">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="E47">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="F47">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="G47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47">
+        <v>3091</v>
+      </c>
+      <c r="J47">
+        <v>0.5584615384615386</v>
+      </c>
+      <c r="K47">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="L47">
+        <v>0.2792307692307693</v>
+      </c>
+      <c r="M47">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="N47">
+        <v>0.7407692307692308</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D48">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="E48">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F48">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48">
+        <v>3545</v>
+      </c>
+      <c r="J48">
+        <v>0.5657142857142857</v>
+      </c>
+      <c r="K48">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="L48">
+        <v>0.2828571428571429</v>
+      </c>
+      <c r="M48">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="N48">
+        <v>0.7471428571428571</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D49">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="E49">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F49">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49">
         <v>3511</v>
       </c>
-      <c r="J45">
+      <c r="J49">
         <v>0.5657142857142857</v>
       </c>
-      <c r="K45">
+      <c r="K49">
         <v>0.9285714285714286</v>
       </c>
-      <c r="L45">
+      <c r="L49">
         <v>0.2828571428571429</v>
       </c>
-      <c r="M45">
+      <c r="M49">
         <v>0.4642857142857143</v>
       </c>
-      <c r="N45">
+      <c r="N49">
         <v>0.7471428571428571</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50">
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D50">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="E50">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="F50">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>40</v>
+      </c>
+      <c r="I50">
+        <v>3511</v>
+      </c>
+      <c r="J50">
+        <v>0.5657142857142857</v>
+      </c>
+      <c r="K50">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="L50">
+        <v>0.2828571428571429</v>
+      </c>
+      <c r="M50">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="N50">
+        <v>0.7471428571428571</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51">
+        <v>0.7796610169491526</v>
+      </c>
+      <c r="B51">
+        <v>0.01694915254237288</v>
+      </c>
+      <c r="C51">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="D51">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="E51">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="F51">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51">
+        <v>3695</v>
+      </c>
+      <c r="J51">
+        <v>0.5705084745762712</v>
+      </c>
+      <c r="K51">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="L51">
+        <v>0.2852542372881356</v>
+      </c>
+      <c r="M51">
+        <v>0.4661016949152542</v>
+      </c>
+      <c r="N51">
+        <v>0.7513559322033898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>